<commit_message>
Further updates to the BoM (Still not ready to be used)
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.2/schematic v0.2_bom.xlsx
+++ b/reference/hardware/v0.2/schematic v0.2_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="355">
   <si>
     <t>QTY</t>
   </si>
@@ -342,15 +342,6 @@
     <t>LED-Red</t>
   </si>
   <si>
-    <t>LED SS 3MM 625NM RED DIFF</t>
-  </si>
-  <si>
-    <t>WP132XID</t>
-  </si>
-  <si>
-    <t>754-1211-ND</t>
-  </si>
-  <si>
     <t>D50,51,52,53</t>
   </si>
   <si>
@@ -387,27 +378,6 @@
     <t>1N4004-TPMSCT-ND</t>
   </si>
   <si>
-    <t>Connectors/Jacks</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>USB-B micro</t>
-  </si>
-  <si>
-    <t>CONN USB MICRO B RECPT SMT R/A</t>
-  </si>
-  <si>
-    <t>FCI</t>
-  </si>
-  <si>
-    <t>10118194-0001LF</t>
-  </si>
-  <si>
-    <t>609-4618-1-ND</t>
-  </si>
-  <si>
     <t>MOV1</t>
   </si>
   <si>
@@ -864,24 +834,9 @@
     <t>U1</t>
   </si>
   <si>
-    <t>MC9S12XDP512</t>
-  </si>
-  <si>
-    <t>IC MCU 512K FLASH 112-LQFP MC9S12XDP512MAL</t>
-  </si>
-  <si>
-    <t>LQFP-112</t>
-  </si>
-  <si>
     <t>Freescale Semiconductor</t>
   </si>
   <si>
-    <t>MC9S12XDP512MAL</t>
-  </si>
-  <si>
-    <t>MC9S12XDP512MAL-ND</t>
-  </si>
-  <si>
     <t>U2,3</t>
   </si>
   <si>
@@ -897,18 +852,6 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>SP900S-0.009-AC-54</t>
-  </si>
-  <si>
-    <t>SILICONE THERMAL PAD TO-220 W/ADH .009" SP9</t>
-  </si>
-  <si>
-    <t>Bergquist</t>
-  </si>
-  <si>
-    <t>BER182-ND</t>
-  </si>
-  <si>
     <t>7721-7PPSG</t>
   </si>
   <si>
@@ -921,15 +864,6 @@
     <t>HS418-ND</t>
   </si>
   <si>
-    <t>MICA PAD AND HARDWARE MOUNTING KIT FOR TO-220</t>
-  </si>
-  <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>4724K-ND</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -969,36 +903,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>MPXA4250AC6U</t>
-  </si>
-  <si>
-    <t>PRESSURE SENS 36.3PSI MAX 8-SOP</t>
-  </si>
-  <si>
-    <t>MPXA4250AC6U-ND</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>FT232RL</t>
-  </si>
-  <si>
-    <t>IC FT232RL USB FS SERIAL UART 28-SSOP</t>
-  </si>
-  <si>
-    <t>28-SSOP</t>
-  </si>
-  <si>
-    <t>FTDI, Future Technology Devices International Ltd</t>
-  </si>
-  <si>
-    <t>FT232RL-REEL</t>
-  </si>
-  <si>
-    <t>768-1007-1-ND</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
@@ -1068,33 +972,6 @@
     <t>296-17623-1-ND</t>
   </si>
   <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>16.0MHz</t>
-  </si>
-  <si>
-    <t>CRYSTAL 16.000 MHZ 20PF 49US -40C to 85C</t>
-  </si>
-  <si>
-    <t>HC-49US</t>
-  </si>
-  <si>
-    <t>ECS Inc</t>
-  </si>
-  <si>
-    <t>ECS-160-20-4DN</t>
-  </si>
-  <si>
-    <t>X192-ND</t>
-  </si>
-  <si>
-    <t>Cost To Manufacture (CTM)</t>
-  </si>
-  <si>
     <t>US Dollars</t>
   </si>
   <si>
@@ -1174,6 +1051,39 @@
   </si>
   <si>
     <t>Not used</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>LED SS 5MM 625NM RED DIFF</t>
+  </si>
+  <si>
+    <t>5mm-LED</t>
+  </si>
+  <si>
+    <t>D9,10,11,12</t>
+  </si>
+  <si>
+    <t>MPX4250AP-ND</t>
+  </si>
+  <si>
+    <t>6-SIP</t>
+  </si>
+  <si>
+    <t>SENSOR ABS PRESS 36.3 PSI MAX</t>
+  </si>
+  <si>
+    <t>MPX4250A</t>
+  </si>
+  <si>
+    <t>AE10011-ND</t>
+  </si>
+  <si>
+    <t>AR08-HZL-TT-R</t>
+  </si>
+  <si>
+    <t>IC SOCKET MACH PIN ST 8POS TIN</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1093,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1208,11 +1118,6 @@
       <name val="Liberation Sans"/>
     </font>
     <font>
-      <sz val="7.5"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -1227,6 +1132,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1279,7 +1195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1305,21 +1221,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -1357,10 +1258,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1382,7 +1283,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1394,10 +1295,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1409,7 +1307,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,19 +1319,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1445,10 +1337,10 @@
     <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1457,20 +1349,27 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1807,10 +1706,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M88"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1829,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1880,14 +1782,14 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="27" thickBot="1">
-      <c r="A3" s="5">
+      <c r="A3" s="33">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>381</v>
+        <v>340</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -2104,14 +2006,14 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="27" thickBot="1">
-      <c r="A9" s="5">
-        <v>2</v>
+      <c r="A9" s="33">
+        <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>382</v>
+        <v>341</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>50</v>
@@ -2291,14 +2193,14 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="27" thickBot="1">
-      <c r="A14" s="5">
-        <v>1</v>
+      <c r="A14" s="33">
+        <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>384</v>
+        <v>343</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>76</v>
@@ -2362,13 +2264,15 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="27" thickBot="1">
-      <c r="A17" s="5">
-        <v>1</v>
+      <c r="A17" s="33">
+        <v>0</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>343</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>82</v>
       </c>
@@ -2405,7 +2309,9 @@
       <c r="B18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>344</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>89</v>
       </c>
@@ -2509,43 +2415,31 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="27" thickBot="1">
-      <c r="A21" s="36">
+    <row r="21" spans="1:13" ht="16" thickBot="1">
+      <c r="A21" s="33">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>383</v>
+        <v>342</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>107</v>
+        <v>345</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="3">
-        <v>13</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="K21" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="L21" s="9">
-        <v>1.35</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="40" thickBot="1">
@@ -2553,29 +2447,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G22" s="3">
         <v>4</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K22" s="8">
         <v>0.2</v>
@@ -2586,18 +2480,20 @@
       <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="40" thickBot="1">
-      <c r="A23" s="5">
-        <v>13</v>
+      <c r="A23" s="33">
+        <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>347</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>91</v>
@@ -2609,10 +2505,10 @@
         <v>103</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K23" s="8">
         <v>0.11</v>
@@ -2638,883 +2534,905 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" ht="16" thickBot="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" ht="27" thickBot="1">
-      <c r="A26" s="12">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:13" ht="16" thickBot="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" ht="27" thickBot="1">
+      <c r="A27" s="33">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="J27" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3">
-        <v>1</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="K27" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" ht="27" thickBot="1">
+      <c r="A28" s="5">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="K26" s="8">
-        <v>0.43</v>
-      </c>
-      <c r="L26" s="9">
-        <v>0.43</v>
-      </c>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" ht="16" thickBot="1">
-      <c r="A27" s="13"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" ht="16" thickBot="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.4</v>
+      </c>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13" ht="27" thickBot="1">
+    <row r="29" spans="1:13" ht="40" thickBot="1">
       <c r="A29" s="5">
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="3" t="s">
-        <v>130</v>
+      <c r="D29" s="3">
+        <v>40</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="G29" s="3">
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="K29" s="8">
-        <v>0.72</v>
+        <v>0.1</v>
       </c>
       <c r="L29" s="9">
-        <v>0.72</v>
+        <v>0.1</v>
       </c>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" ht="27" thickBot="1">
+    <row r="30" spans="1:13" ht="40" thickBot="1">
       <c r="A30" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G30" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K30" s="8">
-        <v>0.2</v>
+        <v>1.58</v>
       </c>
       <c r="L30" s="9">
-        <v>0.4</v>
+        <v>11.07</v>
       </c>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:13" ht="40" thickBot="1">
-      <c r="A31" s="5">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>143</v>
-      </c>
+    <row r="31" spans="1:13" ht="16" thickBot="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="3">
-        <v>40</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" ht="16" thickBot="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" ht="27" thickBot="1">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K31" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="L31" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" ht="40" thickBot="1">
-      <c r="A32" s="5">
+      <c r="E33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K33" s="9">
+        <v>3.11</v>
+      </c>
+      <c r="L33" s="9">
+        <v>3.11</v>
+      </c>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" ht="40" thickBot="1">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K34" s="9">
+        <v>2.13</v>
+      </c>
+      <c r="L34" s="9">
+        <v>2.13</v>
+      </c>
+      <c r="M34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" ht="16" thickBot="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" ht="16" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+    </row>
+    <row r="37" spans="1:13" ht="27" thickBot="1">
+      <c r="A37" s="5">
+        <v>8</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="3">
+        <v>8</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="L37" s="9">
+        <v>14</v>
+      </c>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" ht="40" thickBot="1">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0.61</v>
+      </c>
+      <c r="L38" s="9">
+        <v>0.61</v>
+      </c>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" ht="16" thickBot="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" ht="16" thickBot="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" ht="27" thickBot="1">
+      <c r="A41" s="5">
         <v>7</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="B41" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3">
         <v>7</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="K32" s="8">
-        <v>1.58</v>
-      </c>
-      <c r="L32" s="9">
-        <v>11.07</v>
-      </c>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" ht="16" thickBot="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" ht="16" thickBot="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" ht="27" thickBot="1">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3">
-        <v>1</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="K35" s="9">
-        <v>3.11</v>
-      </c>
-      <c r="L35" s="9">
-        <v>3.11</v>
-      </c>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" ht="40" thickBot="1">
-      <c r="A36" s="5">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="K36" s="9">
-        <v>2.13</v>
-      </c>
-      <c r="L36" s="9">
-        <v>2.13</v>
-      </c>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" ht="16" thickBot="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" ht="16" thickBot="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" ht="27" thickBot="1">
-      <c r="A39" s="5">
-        <v>8</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="H41" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K41" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L41" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" ht="53" thickBot="1">
+      <c r="A42" s="5">
+        <v>4</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="3">
-        <v>8</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="K39" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="L39" s="9">
-        <v>14</v>
-      </c>
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="1:13" ht="40" thickBot="1">
-      <c r="A40" s="5">
-        <v>1</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G40" s="3">
-        <v>1</v>
-      </c>
-      <c r="H40" s="3" t="s">
+      <c r="E42" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="J40" s="2" t="s">
+      <c r="F42" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="K40" s="8">
-        <v>0.61</v>
-      </c>
-      <c r="L40" s="9">
-        <v>0.61</v>
-      </c>
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" ht="16" thickBot="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" ht="16" thickBot="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4" t="s">
+      <c r="G42" s="14">
+        <v>4</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" ht="27" thickBot="1">
+      <c r="I42" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="K42" s="16">
+        <v>0.23</v>
+      </c>
+      <c r="L42" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="M42" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="40" thickBot="1">
       <c r="A43" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="J43" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="K43" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L43" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" ht="27" thickBot="1">
+      <c r="A44" s="5">
+        <v>32</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3">
+        <v>32</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="K44" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L44" s="9">
+        <v>1.82</v>
+      </c>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" ht="40" thickBot="1">
+      <c r="A45" s="28">
+        <v>17</v>
+      </c>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="30">
+        <v>17</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="K45" s="31">
         <v>0.08</v>
       </c>
-      <c r="L43" s="9">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" ht="53" thickBot="1">
-      <c r="A44" s="5">
-        <v>4</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="G44" s="15">
-        <v>4</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="K44" s="17">
-        <v>0.23</v>
-      </c>
-      <c r="L44" s="17">
-        <v>0.92</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="40" thickBot="1">
-      <c r="A45" s="5">
-        <v>1</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="L45" s="32">
+        <v>1.39</v>
+      </c>
+      <c r="M45" s="29"/>
+    </row>
+    <row r="46" spans="1:13" ht="16" thickBot="1">
+      <c r="A46" s="5">
+        <v>17</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="3" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E46" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3">
-        <v>1</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="K45" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L45" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="46" spans="1:13" ht="27" thickBot="1">
-      <c r="A46" s="5">
-        <v>32</v>
-      </c>
-      <c r="B46" s="4" t="s">
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" ht="40" thickBot="1">
+      <c r="A47" s="5">
+        <v>9</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="C47" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D47" s="3">
+        <v>470</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F47" s="3"/>
+      <c r="G47" s="3">
+        <v>9</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3">
-        <v>32</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I46" s="3" t="s">
+      <c r="I47" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="J46" s="11" t="s">
+      <c r="J47" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K46" s="8">
-        <v>0.06</v>
-      </c>
-      <c r="L46" s="9">
-        <v>1.82</v>
-      </c>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" ht="40" thickBot="1">
-      <c r="A47" s="31">
-        <v>17</v>
-      </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>375</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="33">
-        <v>17</v>
-      </c>
-      <c r="H47" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="J47" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="K47" s="34">
-        <v>0.08</v>
-      </c>
-      <c r="L47" s="35">
-        <v>1.39</v>
-      </c>
-      <c r="M47" s="32"/>
-    </row>
-    <row r="48" spans="1:13" ht="16" thickBot="1">
+      <c r="K47" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="L47" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" ht="53" thickBot="1">
       <c r="A48" s="5">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="4" t="s">
+        <v>331</v>
+      </c>
       <c r="D48" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="4"/>
-    </row>
-    <row r="49" spans="1:13" ht="40" thickBot="1">
-      <c r="A49" s="5">
-        <v>9</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="F48" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="3">
+        <v>3</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D49" s="3">
-        <v>470</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="J48" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3">
-        <v>9</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="K48" s="8">
+        <v>1.92</v>
+      </c>
+      <c r="L48" s="9">
+        <v>5.76</v>
+      </c>
+      <c r="M48" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="I49" s="10" t="s">
+    </row>
+    <row r="49" spans="1:13" ht="53" thickBot="1">
+      <c r="A49" s="3">
+        <v>0</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="C49" s="17"/>
+      <c r="D49" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E49" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="K49" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="L49" s="9">
-        <v>0.95</v>
-      </c>
-      <c r="M49" s="4"/>
+      <c r="F49" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G49" s="18">
+        <v>0</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="J49" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="K49" s="20">
+        <v>1.29</v>
+      </c>
+      <c r="L49" s="20">
+        <v>0</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="50" spans="1:13" ht="53" thickBot="1">
-      <c r="A50" s="5">
-        <v>3</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G50" s="3">
-        <v>3</v>
-      </c>
-      <c r="H50" s="3" t="s">
+      <c r="A50" s="3">
+        <v>0</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="C50" s="17"/>
+      <c r="D50" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="E50" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="K50" s="8">
-        <v>1.92</v>
-      </c>
-      <c r="L50" s="9">
-        <v>5.76</v>
-      </c>
-      <c r="M50" s="4" t="s">
+      <c r="F50" s="18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="53" thickBot="1">
+      <c r="G50" s="18">
+        <v>0</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="J50" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="K50" s="20">
+        <v>1.29</v>
+      </c>
+      <c r="L50" s="20">
+        <v>0</v>
+      </c>
+      <c r="M50" s="17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="66" thickBot="1">
       <c r="A51" s="3">
         <v>0</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="G51" s="19">
+      <c r="B51" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="G51" s="18">
         <v>0</v>
       </c>
-      <c r="H51" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="J51" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="K51" s="21">
-        <v>1.29</v>
-      </c>
-      <c r="L51" s="21">
+      <c r="H51" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="J51" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="K51" s="20">
+        <v>0.44</v>
+      </c>
+      <c r="L51" s="20">
         <v>0</v>
       </c>
-      <c r="M51" s="18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="53" thickBot="1">
-      <c r="A52" s="3">
-        <v>0</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="F52" s="19" t="s">
+      <c r="M51" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="G52" s="19">
-        <v>0</v>
-      </c>
-      <c r="H52" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="I52" s="19" t="s">
+    </row>
+    <row r="52" spans="1:13" ht="40" thickBot="1">
+      <c r="A52" s="5">
+        <v>1</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="J52" s="20" t="s">
+      <c r="C52" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="K52" s="21">
-        <v>1.29</v>
-      </c>
-      <c r="L52" s="21">
-        <v>0</v>
-      </c>
-      <c r="M52" s="18" t="s">
+      <c r="E52" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="66" thickBot="1">
-      <c r="A53" s="3">
-        <v>0</v>
-      </c>
-      <c r="B53" s="18" t="s">
+      <c r="F52" s="3"/>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="19" t="s">
+      <c r="J52" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="K52" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L52" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M52" s="4"/>
+    </row>
+    <row r="53" spans="1:13" ht="40" thickBot="1">
+      <c r="A53" s="5">
+        <v>1</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="C53" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="19">
-        <v>0</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="I53" s="19" t="s">
+      <c r="E53" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J53" s="20" t="s">
+      <c r="F53" s="3"/>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I53" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K53" s="21">
-        <v>0.44</v>
-      </c>
-      <c r="L53" s="21">
-        <v>0</v>
-      </c>
-      <c r="M53" s="18" t="s">
+      <c r="J53" s="11" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="40" thickBot="1">
+      <c r="K53" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L53" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M53" s="4"/>
+    </row>
+    <row r="54" spans="1:13" ht="27" thickBot="1">
       <c r="A54" s="5">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>241</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>242</v>
@@ -3524,10 +3442,10 @@
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>244</v>
@@ -3536,300 +3454,300 @@
         <v>245</v>
       </c>
       <c r="K54" s="8">
-        <v>0.55000000000000004</v>
+        <v>0.06</v>
       </c>
       <c r="L54" s="9">
-        <v>0.55000000000000004</v>
+        <v>0.97</v>
       </c>
       <c r="M54" s="4"/>
     </row>
-    <row r="55" spans="1:13" ht="40" thickBot="1">
+    <row r="55" spans="1:13" ht="27" thickBot="1">
       <c r="A55" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>246</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="D55" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D55" s="3">
+        <v>160</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I55" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="J55" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="J55" s="11" t="s">
+      <c r="K55" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="L55" s="9">
+        <v>1.08</v>
+      </c>
+      <c r="M55" s="4"/>
+    </row>
+    <row r="56" spans="1:13" ht="40" thickBot="1">
+      <c r="A56" s="5">
+        <v>2</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="K55" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L55" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="1:13" ht="27" thickBot="1">
-      <c r="A56" s="5">
-        <v>17</v>
-      </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="F56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G56" s="3">
+        <v>2</v>
+      </c>
+      <c r="H56" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="I56" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3">
-        <v>17</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I56" s="3" t="s">
+      <c r="J56" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="J56" s="11" t="s">
+      <c r="K56" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="L56" s="9">
+        <v>1.02</v>
+      </c>
+      <c r="M56" s="4"/>
+    </row>
+    <row r="57" spans="1:13" ht="53" thickBot="1">
+      <c r="A57" s="5">
+        <v>1</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="K56" s="8">
-        <v>0.06</v>
-      </c>
-      <c r="L56" s="9">
-        <v>0.97</v>
-      </c>
-      <c r="M56" s="4"/>
-    </row>
-    <row r="57" spans="1:13" ht="27" thickBot="1">
-      <c r="A57" s="5">
-        <v>4</v>
-      </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="4"/>
+      <c r="D57" s="3">
+        <v>330</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D57" s="3">
-        <v>160</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="F57" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3">
-        <v>4</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="J57" s="3" t="s">
+      <c r="J57" s="10" t="s">
         <v>259</v>
       </c>
       <c r="K57" s="8">
-        <v>0.27</v>
+        <v>0.63</v>
       </c>
       <c r="L57" s="9">
-        <v>1.08</v>
+        <v>0.63</v>
       </c>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13" ht="40" thickBot="1">
+    <row r="58" spans="1:13" ht="53" thickBot="1">
       <c r="A58" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>260</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="E58" s="10" t="s">
+      <c r="D58" s="3">
+        <v>604</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>261</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I58" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="I58" s="10" t="s">
+      <c r="J58" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J58" s="3" t="s">
+      <c r="K58" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="L58" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="M58" s="4"/>
+    </row>
+    <row r="59" spans="1:13" ht="40" thickBot="1">
+      <c r="A59" s="5">
+        <v>4</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="K58" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="L58" s="9">
-        <v>1.02</v>
-      </c>
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:13" ht="53" thickBot="1">
-      <c r="A59" s="5">
-        <v>1</v>
-      </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4"/>
+      <c r="D59" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="3">
-        <v>330</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>266</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G59" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H59" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I59" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="J59" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="J59" s="10" t="s">
+      <c r="K59" s="21"/>
+      <c r="L59" s="9">
+        <v>0</v>
+      </c>
+      <c r="M59" s="4"/>
+    </row>
+    <row r="60" spans="1:13" ht="16" thickBot="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="4"/>
+    </row>
+    <row r="61" spans="1:13" ht="16" thickBot="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="K59" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="L59" s="9">
-        <v>0.63</v>
-      </c>
-      <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="1:13" ht="53" thickBot="1">
-      <c r="A60" s="5">
-        <v>1</v>
-      </c>
-      <c r="B60" s="4" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="4"/>
+    </row>
+    <row r="62" spans="1:13" ht="40" thickBot="1">
+      <c r="A62" s="5">
+        <v>1</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="3">
-        <v>604</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G60" s="3">
-        <v>1</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="I60" s="10" t="s">
+      <c r="D62" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="3">
+        <v>2</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="K62" s="8">
+        <v>1.68</v>
+      </c>
+      <c r="L62" s="9">
+        <v>3.36</v>
+      </c>
+      <c r="M62" s="4"/>
+    </row>
+    <row r="63" spans="1:13" ht="27" thickBot="1">
+      <c r="A63" s="5">
+        <v>2</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="J60" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="K60" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="L60" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="M60" s="4"/>
-    </row>
-    <row r="61" spans="1:13" ht="40" thickBot="1">
-      <c r="A61" s="5">
-        <v>4</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G61" s="3">
-        <v>4</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="I61" s="3" t="s">
+      <c r="C63" s="4"/>
+      <c r="D63" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="J61" s="10" t="s">
+      <c r="E63" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="K61" s="22"/>
-      <c r="L61" s="9">
-        <v>0</v>
-      </c>
-      <c r="M61" s="4"/>
-    </row>
-    <row r="62" spans="1:13" ht="16" thickBot="1">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="4"/>
-    </row>
-    <row r="63" spans="1:13" ht="16" thickBot="1">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4" t="s">
+      <c r="F63" s="3"/>
+      <c r="G63" s="3">
+        <v>2</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
+      <c r="I63" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K63" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="L63" s="9">
+        <v>0.46</v>
+      </c>
       <c r="M63" s="4"/>
     </row>
     <row r="64" spans="1:13" ht="40" thickBot="1">
@@ -3837,41 +3755,41 @@
         <v>1</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E64" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G64" s="3">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I64" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G64" s="3">
-        <v>1</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="J64" s="23" t="s">
+      <c r="J64" s="11" t="s">
         <v>286</v>
       </c>
       <c r="K64" s="9">
-        <v>23.53</v>
+        <v>3.59</v>
       </c>
       <c r="L64" s="9">
-        <v>23.53</v>
+        <v>3.59</v>
       </c>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" ht="40" thickBot="1">
+    <row r="65" spans="1:13" ht="27" thickBot="1">
       <c r="A65" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>287</v>
@@ -3887,92 +3805,94 @@
         <v>290</v>
       </c>
       <c r="G65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H65" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I65" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="J65" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="K65" s="8">
-        <v>1.68</v>
+      <c r="J65" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K65" s="9">
+        <v>1.73</v>
       </c>
       <c r="L65" s="9">
-        <v>3.36</v>
+        <v>1.73</v>
       </c>
       <c r="M65" s="4"/>
     </row>
     <row r="66" spans="1:13" ht="40" thickBot="1">
-      <c r="A66" s="5">
-        <v>2</v>
+      <c r="A66" s="33">
+        <v>1</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="3" t="s">
-        <v>292</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F66" s="3"/>
+        <v>350</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>349</v>
+      </c>
       <c r="G66" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="K66" s="8">
-        <v>0.18</v>
+        <v>271</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="K66" s="9">
+        <v>16.37</v>
       </c>
       <c r="L66" s="9">
-        <v>0.36</v>
+        <v>16.37</v>
       </c>
       <c r="M66" s="4"/>
     </row>
     <row r="67" spans="1:13" ht="27" thickBot="1">
       <c r="A67" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="F67" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G67" s="3">
+        <v>1</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3">
-        <v>2</v>
-      </c>
-      <c r="H67" s="3" t="s">
+      <c r="I67" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="J67" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="I67" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="K67" s="8">
-        <v>0.23</v>
+        <v>3.63</v>
       </c>
       <c r="L67" s="9">
-        <v>0.46</v>
+        <v>3.63</v>
       </c>
       <c r="M67" s="4"/>
     </row>
@@ -3981,107 +3901,107 @@
         <v>2</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="C68" s="4"/>
-      <c r="D68" s="3">
-        <v>4724</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F68" s="3"/>
+      <c r="E68" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="G68" s="3">
         <v>2</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="I68" s="3">
-        <v>4724</v>
-      </c>
-      <c r="J68" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K68" s="9">
-        <v>1.94</v>
+      <c r="I68" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="K68" s="8">
+        <v>1.98</v>
       </c>
       <c r="L68" s="9">
-        <v>3.88</v>
+        <v>3.96</v>
       </c>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" ht="40" thickBot="1">
+    <row r="69" spans="1:13" ht="27" thickBot="1">
       <c r="A69" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E69" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G69" s="3">
+        <v>2</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I69" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="G69" s="3">
-        <v>1</v>
-      </c>
-      <c r="H69" s="3" t="s">
+      <c r="J69" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="J69" s="11" t="s">
+      <c r="K69" s="8">
+        <v>1.96</v>
+      </c>
+      <c r="L69" s="9">
+        <v>3.92</v>
+      </c>
+      <c r="M69" s="4"/>
+    </row>
+    <row r="70" spans="1:13" ht="40" thickBot="1">
+      <c r="A70" s="5">
+        <v>1</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="K69" s="9">
-        <v>3.59</v>
-      </c>
-      <c r="L69" s="9">
-        <v>3.59</v>
-      </c>
-      <c r="M69" s="4"/>
-    </row>
-    <row r="70" spans="1:13" ht="27" thickBot="1">
-      <c r="A70" s="5">
-        <v>1</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>309</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="F70" s="3"/>
+      <c r="G70" s="3">
+        <v>1</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G70" s="3">
-        <v>1</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I70" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>314</v>
-      </c>
       <c r="K70" s="9">
-        <v>1.73</v>
+        <v>12.55</v>
       </c>
       <c r="L70" s="9">
-        <v>1.73</v>
+        <v>12.55</v>
       </c>
       <c r="M70" s="4"/>
     </row>
@@ -4090,255 +4010,169 @@
         <v>1</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G71" s="3">
+        <v>1</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G71" s="3">
-        <v>1</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="K71" s="9">
-        <v>16.37</v>
+      <c r="K71" s="8">
+        <v>0.72</v>
       </c>
       <c r="L71" s="9">
-        <v>16.37</v>
+        <v>0.72</v>
       </c>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" ht="56" thickBot="1">
-      <c r="A72" s="5">
-        <v>1</v>
-      </c>
-      <c r="B72" s="4" t="s">
+    <row r="72" spans="1:13" ht="27" thickBot="1">
+      <c r="A72" s="3">
+        <v>1</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="J72" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="4"/>
+    </row>
+    <row r="73" spans="1:13" ht="16" thickBot="1">
+      <c r="A73" s="3"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+    </row>
+    <row r="74" spans="1:13" ht="66" thickBot="1">
+      <c r="A74" s="5">
+        <v>1</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="3" t="s">
+      <c r="C74" s="4"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="F74" s="3"/>
+      <c r="G74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="I74" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="G72" s="3">
-        <v>1</v>
-      </c>
-      <c r="H72" s="24" t="s">
+      <c r="J74" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="K74" s="9">
+        <v>14.99</v>
+      </c>
+      <c r="L74" s="9">
+        <v>14.99</v>
+      </c>
+      <c r="M74" s="23"/>
+    </row>
+    <row r="75" spans="1:13" ht="16" thickBot="1">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="23"/>
+      <c r="M75" s="23"/>
+    </row>
+    <row r="76" spans="1:13" ht="16" thickBot="1">
+      <c r="A76" s="3"/>
+      <c r="B76" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="J72" s="11" t="s">
+      <c r="C76" s="4"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="4"/>
+    </row>
+    <row r="77" spans="1:13" ht="27" thickBot="1">
+      <c r="A77" s="5">
+        <v>1</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>325</v>
-      </c>
-      <c r="K72" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="L72" s="9">
-        <v>4.5</v>
-      </c>
-      <c r="M72" s="4"/>
-    </row>
-    <row r="73" spans="1:13" ht="27" thickBot="1">
-      <c r="A73" s="5">
-        <v>1</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G73" s="3">
-        <v>1</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K73" s="8">
-        <v>3.63</v>
-      </c>
-      <c r="L73" s="9">
-        <v>3.63</v>
-      </c>
-      <c r="M73" s="4"/>
-    </row>
-    <row r="74" spans="1:13" ht="27" thickBot="1">
-      <c r="A74" s="5">
-        <v>2</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G74" s="3">
-        <v>2</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="K74" s="8">
-        <v>1.98</v>
-      </c>
-      <c r="L74" s="9">
-        <v>3.96</v>
-      </c>
-      <c r="M74" s="4"/>
-    </row>
-    <row r="75" spans="1:13" ht="27" thickBot="1">
-      <c r="A75" s="5">
-        <v>2</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G75" s="3">
-        <v>2</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="K75" s="8">
-        <v>1.96</v>
-      </c>
-      <c r="L75" s="9">
-        <v>3.92</v>
-      </c>
-      <c r="M75" s="4"/>
-    </row>
-    <row r="76" spans="1:13" ht="40" thickBot="1">
-      <c r="A76" s="5">
-        <v>1</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3">
-        <v>1</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="K76" s="9">
-        <v>12.55</v>
-      </c>
-      <c r="L76" s="9">
-        <v>12.55</v>
-      </c>
-      <c r="M76" s="4"/>
-    </row>
-    <row r="77" spans="1:13" ht="40" thickBot="1">
-      <c r="A77" s="5">
-        <v>1</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>344</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>347</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="3">
         <v>1</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="K77" s="8">
-        <v>0.72</v>
+        <v>327</v>
+      </c>
+      <c r="J77" s="3"/>
+      <c r="K77" s="9">
+        <v>10</v>
       </c>
       <c r="L77" s="9">
-        <v>0.72</v>
+        <v>10</v>
       </c>
       <c r="M77" s="4"/>
     </row>
@@ -4357,237 +4191,34 @@
       <c r="L78" s="3"/>
       <c r="M78" s="4"/>
     </row>
-    <row r="79" spans="1:13" ht="16" thickBot="1">
+    <row r="79" spans="1:13" ht="53" thickBot="1">
       <c r="A79" s="3"/>
-      <c r="B79" s="4" t="s">
-        <v>349</v>
-      </c>
+      <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="4"/>
-    </row>
-    <row r="80" spans="1:13" ht="27" thickBot="1">
-      <c r="A80" s="5">
-        <v>1</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="G80" s="3">
-        <v>1</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="J80" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="K80" s="8">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="L80" s="9">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="M80" s="4"/>
-    </row>
-    <row r="81" spans="1:13" ht="53" thickBot="1">
-      <c r="A81" s="3"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="28" t="s">
-        <v>357</v>
-      </c>
-      <c r="J81" s="29"/>
-      <c r="K81" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="L81" s="25">
-        <v>171.09620000000001</v>
-      </c>
-      <c r="M81" s="26" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="16" thickBot="1">
-      <c r="A82" s="3"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="25"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="26"/>
-      <c r="M82" s="26"/>
-    </row>
-    <row r="83" spans="1:13" ht="66" thickBot="1">
-      <c r="A83" s="5">
-        <v>1</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3">
-        <v>1</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="J83" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="K83" s="9">
-        <v>14.99</v>
-      </c>
-      <c r="L83" s="9">
-        <v>14.99</v>
-      </c>
-      <c r="M83" s="26"/>
-    </row>
-    <row r="84" spans="1:13" ht="16" thickBot="1">
-      <c r="A84" s="3"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="25"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="26"/>
-      <c r="M84" s="26"/>
-    </row>
-    <row r="85" spans="1:13" ht="16" thickBot="1">
-      <c r="A85" s="3"/>
-      <c r="B85" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="4"/>
-    </row>
-    <row r="86" spans="1:13" ht="27" thickBot="1">
-      <c r="A86" s="5">
-        <v>1</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3">
-        <v>1</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="J86" s="3"/>
-      <c r="K86" s="9">
-        <v>10</v>
-      </c>
-      <c r="L86" s="9">
-        <v>10</v>
-      </c>
-      <c r="M86" s="4"/>
-    </row>
-    <row r="87" spans="1:13" ht="16" thickBot="1">
-      <c r="A87" s="3"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="4"/>
-    </row>
-    <row r="88" spans="1:13" ht="53" thickBot="1">
-      <c r="A88" s="3"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="J88" s="29"/>
-      <c r="K88" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="L88" s="27">
+      <c r="G79" s="12"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="J79" s="26"/>
+      <c r="K79" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L79" s="24">
         <v>196.09</v>
       </c>
-      <c r="M88" s="26" t="s">
-        <v>359</v>
+      <c r="M79" s="23" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I88:J88"/>
+  <mergeCells count="1">
+    <mergeCell ref="I79:J79"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1"/>
     <hyperlink ref="J9" r:id="rId2"/>
@@ -4598,31 +4229,28 @@
     <hyperlink ref="J17" r:id="rId7"/>
     <hyperlink ref="J19" r:id="rId8"/>
     <hyperlink ref="J20" r:id="rId9"/>
-    <hyperlink ref="J21" r:id="rId10"/>
-    <hyperlink ref="J29" r:id="rId11"/>
-    <hyperlink ref="J35" r:id="rId12"/>
-    <hyperlink ref="J36" r:id="rId13"/>
-    <hyperlink ref="J43" r:id="rId14"/>
+    <hyperlink ref="J27" r:id="rId10"/>
+    <hyperlink ref="J33" r:id="rId11"/>
+    <hyperlink ref="J34" r:id="rId12"/>
+    <hyperlink ref="J41" r:id="rId13"/>
+    <hyperlink ref="J42" r:id="rId14"/>
     <hyperlink ref="J44" r:id="rId15"/>
-    <hyperlink ref="J46" r:id="rId16"/>
-    <hyperlink ref="J50" r:id="rId17"/>
-    <hyperlink ref="J51" r:id="rId18"/>
-    <hyperlink ref="J52" r:id="rId19"/>
-    <hyperlink ref="J53" r:id="rId20"/>
-    <hyperlink ref="J54" r:id="rId21"/>
-    <hyperlink ref="J55" r:id="rId22"/>
-    <hyperlink ref="J56" r:id="rId23"/>
-    <hyperlink ref="J64" r:id="rId24"/>
-    <hyperlink ref="J69" r:id="rId25"/>
-    <hyperlink ref="J72" r:id="rId26"/>
-    <hyperlink ref="J80" r:id="rId27"/>
-    <hyperlink ref="J83" r:id="rId28"/>
+    <hyperlink ref="J48" r:id="rId16"/>
+    <hyperlink ref="J49" r:id="rId17"/>
+    <hyperlink ref="J50" r:id="rId18"/>
+    <hyperlink ref="J51" r:id="rId19"/>
+    <hyperlink ref="J52" r:id="rId20"/>
+    <hyperlink ref="J53" r:id="rId21"/>
+    <hyperlink ref="J54" r:id="rId22"/>
+    <hyperlink ref="J64" r:id="rId23"/>
+    <hyperlink ref="J74" r:id="rId24"/>
+    <hyperlink ref="J66" r:id="rId25"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="36" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Further updates to the BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.2/schematic v0.2_bom.xlsx
+++ b/reference/hardware/v0.2/schematic v0.2_bom.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,8 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Josh Stewart</author>
+  </authors>
+  <commentList>
+    <comment ref="C46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Josh Stewart:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional 3rd one for a spare ADC</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="299">
   <si>
     <t>QTY</t>
   </si>
@@ -549,42 +583,6 @@
     <t>10.0KXBK-ND</t>
   </si>
   <si>
-    <t>R16,17,18,19</t>
-  </si>
-  <si>
-    <t>RES 10.0K OHM 1/2W 1% METAL FILM</t>
-  </si>
-  <si>
-    <t>If using VR inputs</t>
-  </si>
-  <si>
-    <t>Vishay/BC Components</t>
-  </si>
-  <si>
-    <t>SFR16S0001002FR500</t>
-  </si>
-  <si>
-    <t>PPC10.0KXCT-ND</t>
-  </si>
-  <si>
-    <t>Only purchase if using VR inputs</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>3.3k</t>
-  </si>
-  <si>
-    <t>RES 3.3K OHM 1/4W 0.1% AXIAL</t>
-  </si>
-  <si>
-    <t>MFP-25BRD52-3K3</t>
-  </si>
-  <si>
-    <t>3.3KADCT-ND</t>
-  </si>
-  <si>
     <t>R7,13,16,17,18,19,21,22,41,42,43,44,45,46,54,56,59,60,70,71,74,77,78,80,81,83,84,87,88,95,104,105</t>
   </si>
   <si>
@@ -654,66 +652,6 @@
     <t>Only purchase if using GM Sensors</t>
   </si>
   <si>
-    <t>R24,25,31 | For most sensors</t>
-  </si>
-  <si>
-    <t>RES 2.43K OHM 0.25W 0.1% METAL FILM</t>
-  </si>
-  <si>
-    <t>For Most Sensors</t>
-  </si>
-  <si>
-    <t>RC55Y-2K43BI</t>
-  </si>
-  <si>
-    <t>985-1046-1-ND</t>
-  </si>
-  <si>
-    <t>Good compromise for most Sensors</t>
-  </si>
-  <si>
-    <t>R24,25,31 | For Ford sensors</t>
-  </si>
-  <si>
-    <t>27.4k</t>
-  </si>
-  <si>
-    <t>RES 27.4K OHM 0.25W 0.1% METAL FILM AXL</t>
-  </si>
-  <si>
-    <t>For Ford Sensors</t>
-  </si>
-  <si>
-    <t>RC55Y-27K4BI</t>
-  </si>
-  <si>
-    <t>985-1069-1-ND</t>
-  </si>
-  <si>
-    <t>Only purchase if using Ford Sensors</t>
-  </si>
-  <si>
-    <t>R24,25,31 | For MOPAR sensors</t>
-  </si>
-  <si>
-    <t>9.1k</t>
-  </si>
-  <si>
-    <t>RES 9.1K OHM 1/4W 0.1% METAL FILM AXL</t>
-  </si>
-  <si>
-    <t>For MOPAR Sensors</t>
-  </si>
-  <si>
-    <t>MFP-25BRD52-9K1</t>
-  </si>
-  <si>
-    <t>9.1KADCT-ND</t>
-  </si>
-  <si>
-    <t>Only purchase if using Mopar Sensors</t>
-  </si>
-  <si>
     <t>R29</t>
   </si>
   <si>
@@ -771,63 +709,6 @@
     <t>160YCT-ND</t>
   </si>
   <si>
-    <t>R106,107</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 1/8W 0.1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>Bourns Inc</t>
-  </si>
-  <si>
-    <t>CRT0805-BY-1002ELF</t>
-  </si>
-  <si>
-    <t>CRT0805-BY-1002ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R108</t>
-  </si>
-  <si>
-    <t>RES 330 OHM 1/8W 0.1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>Panasonic Electronic Components</t>
-  </si>
-  <si>
-    <t>ERA-6AEB331V</t>
-  </si>
-  <si>
-    <t>P330DACT-ND</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>RES 604 OHM 1/8W 0.1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>ERA-6AEB6040V</t>
-  </si>
-  <si>
-    <t>P604DACT-ND</t>
-  </si>
-  <si>
-    <t>R64,65,79,85</t>
-  </si>
-  <si>
-    <t>2.4k</t>
-  </si>
-  <si>
-    <t>RES 2.4k OHM 1/8W 1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>RMCF0805FT2K40</t>
-  </si>
-  <si>
-    <t>RMCF0805FT2K40CT-ND</t>
-  </si>
-  <si>
     <t>ICs</t>
   </si>
   <si>
@@ -864,24 +745,6 @@
     <t>HS418-ND</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>MAX9926UAEE+</t>
-  </si>
-  <si>
-    <t>IC SENSOR INTERFACE VARI 16-QSOP</t>
-  </si>
-  <si>
-    <t>16-QSOP</t>
-  </si>
-  <si>
-    <t>Maxim Integrated Products</t>
-  </si>
-  <si>
-    <t>MAX9926UAEE+-ND</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -1084,6 +947,9 @@
   </si>
   <si>
     <t>IC SOCKET MACH PIN ST 8POS TIN</t>
+  </si>
+  <si>
+    <t>R39, 40</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +959,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1144,8 +1010,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1161,18 +1040,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00AE00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94BD5E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,7 +1130,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1301,33 +1168,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1337,16 +1177,10 @@
     <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1355,13 +1189,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1370,6 +1204,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1705,14 +1545,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1731,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>329</v>
+        <v>272</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1782,14 +1622,14 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="27" thickBot="1">
-      <c r="A3" s="33">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -2006,14 +1846,14 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="27" thickBot="1">
-      <c r="A9" s="33">
+      <c r="A9" s="22">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>341</v>
+        <v>284</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>50</v>
@@ -2193,14 +2033,14 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="27" thickBot="1">
-      <c r="A14" s="33">
+      <c r="A14" s="22">
         <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>76</v>
@@ -2264,14 +2104,14 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="27" thickBot="1">
-      <c r="A17" s="33">
+      <c r="A17" s="22">
         <v>0</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>343</v>
+        <v>286</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>82</v>
@@ -2310,7 +2150,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>344</v>
+        <v>287</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>89</v>
@@ -2416,23 +2256,23 @@
       <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="16" thickBot="1">
-      <c r="A21" s="33">
+      <c r="A21" s="22">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>342</v>
+        <v>285</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>106</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>345</v>
+        <v>288</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>346</v>
+        <v>289</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2480,14 +2320,14 @@
       <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="40" thickBot="1">
-      <c r="A23" s="33">
+      <c r="A23" s="22">
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>347</v>
+        <v>290</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>115</v>
@@ -2564,7 +2404,7 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="27" thickBot="1">
-      <c r="A27" s="33">
+      <c r="A27" s="22">
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -2852,7 +2692,7 @@
       <c r="B37" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="27"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="10" t="s">
         <v>159</v>
       </c>
@@ -2958,7 +2798,9 @@
       <c r="B41" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>298</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>171</v>
       </c>
@@ -2986,405 +2828,357 @@
       </c>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="1:13" ht="53" thickBot="1">
+    <row r="42" spans="1:13" ht="27" thickBot="1">
       <c r="A42" s="5">
-        <v>4</v>
-      </c>
-      <c r="B42" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="E42" s="14" t="s">
+      <c r="C42" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="E42" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="14">
-        <v>4</v>
-      </c>
-      <c r="H42" s="14" t="s">
+      <c r="F42" s="3"/>
+      <c r="G42" s="3">
+        <v>32</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="J42" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="J42" s="15" t="s">
+      <c r="K42" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L42" s="9">
+        <v>1.82</v>
+      </c>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" ht="40" thickBot="1">
+      <c r="A43" s="17">
+        <v>17</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="19">
+        <v>17</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="K43" s="20">
+        <v>0.08</v>
+      </c>
+      <c r="L43" s="21">
+        <v>1.39</v>
+      </c>
+      <c r="M43" s="18"/>
+    </row>
+    <row r="44" spans="1:13" ht="16" thickBot="1">
+      <c r="A44" s="5">
+        <v>17</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="K42" s="16">
-        <v>0.23</v>
-      </c>
-      <c r="L42" s="16">
-        <v>0.92</v>
-      </c>
-      <c r="M42" s="13" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="40" thickBot="1">
-      <c r="A43" s="5">
-        <v>1</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="E44" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3">
-        <v>1</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I43" s="3" t="s">
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" ht="40" thickBot="1">
+      <c r="A45" s="5">
+        <v>9</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="C45" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D45" s="3">
+        <v>470</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K43" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" ht="27" thickBot="1">
-      <c r="A44" s="5">
-        <v>32</v>
-      </c>
-      <c r="B44" s="4" t="s">
+      <c r="F45" s="3"/>
+      <c r="G45" s="3">
+        <v>9</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="I45" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="J45" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3">
-        <v>32</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I44" s="3" t="s">
+      <c r="K45" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" ht="53" thickBot="1">
+      <c r="A46" s="22">
+        <v>3</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J44" s="11" t="s">
+      <c r="C46" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="K44" s="8">
-        <v>0.06</v>
-      </c>
-      <c r="L44" s="9">
-        <v>1.82</v>
-      </c>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" ht="40" thickBot="1">
-      <c r="A45" s="28">
-        <v>17</v>
-      </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29" t="s">
-        <v>336</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>334</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="30">
-        <v>17</v>
-      </c>
-      <c r="H45" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="I45" s="10" t="s">
+      <c r="E46" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G46" s="3">
+        <v>3</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J46" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="K45" s="31">
-        <v>0.08</v>
-      </c>
-      <c r="L45" s="32">
-        <v>1.39</v>
-      </c>
-      <c r="M45" s="29"/>
-    </row>
-    <row r="46" spans="1:13" ht="16" thickBot="1">
-      <c r="A46" s="5">
-        <v>17</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="4"/>
+      <c r="K46" s="8">
+        <v>1.92</v>
+      </c>
+      <c r="L46" s="9">
+        <v>5.76</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="47" spans="1:13" ht="40" thickBot="1">
-      <c r="A47" s="5">
-        <v>9</v>
+      <c r="A47" s="22">
+        <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D47" s="3">
-        <v>470</v>
+        <v>275</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="J47" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>202</v>
       </c>
+      <c r="J47" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="K47" s="8">
-        <v>0.11</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L47" s="9">
-        <v>0.95</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" ht="53" thickBot="1">
-      <c r="A48" s="5">
-        <v>3</v>
+    <row r="48" spans="1:13" ht="40" thickBot="1">
+      <c r="A48" s="22">
+        <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>331</v>
+        <v>276</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F48" s="3" t="s">
         <v>206</v>
       </c>
+      <c r="F48" s="3"/>
       <c r="G48" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H48" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="J48" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="J48" s="11" t="s">
+      <c r="K48" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L48" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="1:13" ht="27" thickBot="1">
+      <c r="A49" s="5">
+        <v>17</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="K48" s="8">
-        <v>1.92</v>
-      </c>
-      <c r="L48" s="9">
-        <v>5.76</v>
-      </c>
-      <c r="M48" s="4" t="s">
+      <c r="C49" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="53" thickBot="1">
-      <c r="A49" s="3">
-        <v>0</v>
-      </c>
-      <c r="B49" s="17" t="s">
+      <c r="E49" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E49" s="18" t="s">
+      <c r="F49" s="3"/>
+      <c r="G49" s="3">
+        <v>17</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="18" t="s">
+      <c r="J49" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="G49" s="18">
-        <v>0</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="I49" s="18" t="s">
+      <c r="K49" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L49" s="9">
+        <v>0.97</v>
+      </c>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="1:13" ht="27" thickBot="1">
+      <c r="A50" s="22">
+        <v>4</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="J49" s="19" t="s">
+      <c r="C50" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50" s="3">
+        <v>160</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="K49" s="20">
-        <v>1.29</v>
-      </c>
-      <c r="L49" s="20">
-        <v>0</v>
-      </c>
-      <c r="M49" s="17" t="s">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3">
+        <v>4</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="53" thickBot="1">
-      <c r="A50" s="3">
-        <v>0</v>
-      </c>
-      <c r="B50" s="17" t="s">
+      <c r="J50" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18" t="s">
+      <c r="K50" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="L50" s="9">
+        <v>1.08</v>
+      </c>
+      <c r="M50" s="4"/>
+    </row>
+    <row r="51" spans="1:13" ht="16" thickBot="1">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="1:13" ht="16" thickBot="1">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="G50" s="18">
-        <v>0</v>
-      </c>
-      <c r="H50" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="I50" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="J50" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="K50" s="20">
-        <v>1.29</v>
-      </c>
-      <c r="L50" s="20">
-        <v>0</v>
-      </c>
-      <c r="M50" s="17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="66" thickBot="1">
-      <c r="A51" s="3">
-        <v>0</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" s="18">
-        <v>0</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="I51" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="J51" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="K51" s="20">
-        <v>0.44</v>
-      </c>
-      <c r="L51" s="20">
-        <v>0</v>
-      </c>
-      <c r="M51" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="40" thickBot="1">
-      <c r="A52" s="5">
-        <v>1</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>233</v>
-      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="3">
-        <v>1</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="K52" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L52" s="9">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
       <c r="M52" s="4"/>
     </row>
     <row r="53" spans="1:13" ht="40" thickBot="1">
@@ -3392,471 +3186,431 @@
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>333</v>
+        <v>219</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="F53" s="3"/>
+        <v>223</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="G53" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="J53" s="11" t="s">
-        <v>240</v>
+        <v>222</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="K53" s="8">
-        <v>0.55000000000000004</v>
+        <v>1.68</v>
       </c>
       <c r="L53" s="9">
-        <v>0.55000000000000004</v>
+        <v>3.36</v>
       </c>
       <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:13" ht="27" thickBot="1">
       <c r="A54" s="5">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>339</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C54" s="4"/>
       <c r="D54" s="3" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>173</v>
+        <v>228</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>245</v>
+        <v>226</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="K54" s="8">
-        <v>0.06</v>
+        <v>0.23</v>
       </c>
       <c r="L54" s="9">
-        <v>0.97</v>
+        <v>0.46</v>
       </c>
       <c r="M54" s="4"/>
     </row>
     <row r="55" spans="1:13" ht="27" thickBot="1">
       <c r="A55" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G55" s="3">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="K55" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="L55" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="M55" s="4"/>
+    </row>
+    <row r="56" spans="1:13" ht="40" thickBot="1">
+      <c r="A56" s="22">
+        <v>1</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="K56" s="9">
+        <v>16.37</v>
+      </c>
+      <c r="L56" s="9">
+        <v>16.37</v>
+      </c>
+      <c r="M56" s="4"/>
+    </row>
+    <row r="57" spans="1:13" ht="27" thickBot="1">
+      <c r="A57" s="5">
+        <v>1</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K57" s="8">
+        <v>3.63</v>
+      </c>
+      <c r="L57" s="9">
+        <v>3.63</v>
+      </c>
+      <c r="M57" s="4"/>
+    </row>
+    <row r="58" spans="1:13" ht="27" thickBot="1">
+      <c r="A58" s="5">
+        <v>2</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G58" s="3">
+        <v>2</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J58" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D55" s="3">
-        <v>160</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="K58" s="8">
+        <v>1.98</v>
+      </c>
+      <c r="L58" s="9">
+        <v>3.96</v>
+      </c>
+      <c r="M58" s="4"/>
+    </row>
+    <row r="59" spans="1:13" ht="27" thickBot="1">
+      <c r="A59" s="5">
+        <v>2</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3">
-        <v>4</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="K55" s="8">
-        <v>0.27</v>
-      </c>
-      <c r="L55" s="9">
-        <v>1.08</v>
-      </c>
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="1:13" ht="40" thickBot="1">
-      <c r="A56" s="5">
-        <v>2</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G56" s="3">
-        <v>2</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="K56" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="L56" s="9">
-        <v>1.02</v>
-      </c>
-      <c r="M56" s="4"/>
-    </row>
-    <row r="57" spans="1:13" ht="53" thickBot="1">
-      <c r="A57" s="5">
-        <v>1</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3">
-        <v>330</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G57" s="3">
-        <v>1</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="K57" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="L57" s="9">
-        <v>0.63</v>
-      </c>
-      <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="1:13" ht="53" thickBot="1">
-      <c r="A58" s="5">
-        <v>1</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="3">
-        <v>604</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G58" s="3">
-        <v>1</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="K58" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:13" ht="40" thickBot="1">
-      <c r="A59" s="5">
-        <v>4</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G59" s="3">
+        <v>2</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="K59" s="8">
+        <v>1.96</v>
+      </c>
+      <c r="L59" s="9">
+        <v>3.92</v>
+      </c>
+      <c r="M59" s="4"/>
+    </row>
+    <row r="60" spans="1:13" ht="40" thickBot="1">
+      <c r="A60" s="5">
+        <v>1</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K60" s="9">
+        <v>12.55</v>
+      </c>
+      <c r="L60" s="9">
+        <v>12.55</v>
+      </c>
+      <c r="M60" s="4"/>
+    </row>
+    <row r="61" spans="1:13" ht="40" thickBot="1">
+      <c r="A61" s="5">
+        <v>1</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K61" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="L61" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="M61" s="4"/>
+    </row>
+    <row r="62" spans="1:13" ht="27" thickBot="1">
+      <c r="A62" s="3">
+        <v>1</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="J62" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="4"/>
+    </row>
+    <row r="63" spans="1:13" ht="16" thickBot="1">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:13" ht="66" thickBot="1">
+      <c r="A64" s="5">
+        <v>1</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I64" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="J64" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="3">
-        <v>4</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="I59" s="3" t="s">
+      <c r="K64" s="9">
+        <v>14.99</v>
+      </c>
+      <c r="L64" s="9">
+        <v>14.99</v>
+      </c>
+      <c r="M64" s="14"/>
+    </row>
+    <row r="65" spans="1:13" ht="16" thickBot="1">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13" ht="16" thickBot="1">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="J59" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="K59" s="21"/>
-      <c r="L59" s="9">
-        <v>0</v>
-      </c>
-      <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="1:13" ht="16" thickBot="1">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="4"/>
-    </row>
-    <row r="61" spans="1:13" ht="16" thickBot="1">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="4"/>
-    </row>
-    <row r="62" spans="1:13" ht="40" thickBot="1">
-      <c r="A62" s="5">
-        <v>1</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="G62" s="3">
-        <v>2</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="J62" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="K62" s="8">
-        <v>1.68</v>
-      </c>
-      <c r="L62" s="9">
-        <v>3.36</v>
-      </c>
-      <c r="M62" s="4"/>
-    </row>
-    <row r="63" spans="1:13" ht="27" thickBot="1">
-      <c r="A63" s="5">
-        <v>2</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3">
-        <v>2</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K63" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="L63" s="9">
-        <v>0.46</v>
-      </c>
-      <c r="M63" s="4"/>
-    </row>
-    <row r="64" spans="1:13" ht="40" thickBot="1">
-      <c r="A64" s="5">
-        <v>1</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="G64" s="3">
-        <v>1</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J64" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="K64" s="9">
-        <v>3.59</v>
-      </c>
-      <c r="L64" s="9">
-        <v>3.59</v>
-      </c>
-      <c r="M64" s="4"/>
-    </row>
-    <row r="65" spans="1:13" ht="27" thickBot="1">
-      <c r="A65" s="5">
-        <v>1</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G65" s="3">
-        <v>1</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="K65" s="9">
-        <v>1.73</v>
-      </c>
-      <c r="L65" s="9">
-        <v>1.73</v>
-      </c>
-      <c r="M65" s="4"/>
-    </row>
-    <row r="66" spans="1:13" ht="40" thickBot="1">
-      <c r="A66" s="33">
-        <v>1</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>351</v>
-      </c>
+      <c r="C66" s="4"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G66" s="3">
-        <v>1</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="I66" s="3"/>
-      <c r="J66" s="34" t="s">
-        <v>348</v>
-      </c>
-      <c r="K66" s="9">
-        <v>16.37</v>
-      </c>
-      <c r="L66" s="9">
-        <v>16.37</v>
-      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="3"/>
       <c r="M66" s="4"/>
     </row>
     <row r="67" spans="1:13" ht="27" thickBot="1">
@@ -3864,359 +3618,73 @@
         <v>1</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>290</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
       <c r="G67" s="3">
         <v>1</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="K67" s="8">
-        <v>3.63</v>
+        <v>270</v>
+      </c>
+      <c r="J67" s="3"/>
+      <c r="K67" s="9">
+        <v>10</v>
       </c>
       <c r="L67" s="9">
-        <v>3.63</v>
+        <v>10</v>
       </c>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" ht="27" thickBot="1">
-      <c r="A68" s="5">
-        <v>2</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>299</v>
-      </c>
+    <row r="68" spans="1:13" ht="16" thickBot="1">
+      <c r="A68" s="3"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G68" s="3">
-        <v>2</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="K68" s="8">
-        <v>1.98</v>
-      </c>
-      <c r="L68" s="9">
-        <v>3.96</v>
-      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" ht="27" thickBot="1">
-      <c r="A69" s="5">
-        <v>2</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>304</v>
-      </c>
+    <row r="69" spans="1:13" ht="53" thickBot="1">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G69" s="3">
-        <v>2</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="K69" s="8">
-        <v>1.96</v>
-      </c>
-      <c r="L69" s="9">
-        <v>3.92</v>
-      </c>
-      <c r="M69" s="4"/>
-    </row>
-    <row r="70" spans="1:13" ht="40" thickBot="1">
-      <c r="A70" s="5">
-        <v>1</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3">
-        <v>1</v>
-      </c>
-      <c r="H70" s="3" t="s">
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="I70" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="K70" s="9">
-        <v>12.55</v>
-      </c>
-      <c r="L70" s="9">
-        <v>12.55</v>
-      </c>
-      <c r="M70" s="4"/>
-    </row>
-    <row r="71" spans="1:13" ht="40" thickBot="1">
-      <c r="A71" s="5">
-        <v>1</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="G71" s="3">
-        <v>1</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="K71" s="8">
-        <v>0.72</v>
-      </c>
-      <c r="L71" s="9">
-        <v>0.72</v>
-      </c>
-      <c r="M71" s="4"/>
-    </row>
-    <row r="72" spans="1:13" ht="27" thickBot="1">
-      <c r="A72" s="3">
-        <v>1</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="35" t="s">
-        <v>354</v>
-      </c>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="J72" s="36" t="s">
-        <v>352</v>
-      </c>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="4"/>
-    </row>
-    <row r="73" spans="1:13" ht="16" thickBot="1">
-      <c r="A73" s="3"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="22"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-    </row>
-    <row r="74" spans="1:13" ht="66" thickBot="1">
-      <c r="A74" s="5">
-        <v>1</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3">
-        <v>1</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="J74" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="K74" s="9">
-        <v>14.99</v>
-      </c>
-      <c r="L74" s="9">
-        <v>14.99</v>
-      </c>
-      <c r="M74" s="23"/>
-    </row>
-    <row r="75" spans="1:13" ht="16" thickBot="1">
-      <c r="A75" s="3"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="23"/>
-      <c r="M75" s="23"/>
-    </row>
-    <row r="76" spans="1:13" ht="16" thickBot="1">
-      <c r="A76" s="3"/>
-      <c r="B76" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="3"/>
-      <c r="M76" s="4"/>
-    </row>
-    <row r="77" spans="1:13" ht="27" thickBot="1">
-      <c r="A77" s="5">
-        <v>1</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3">
-        <v>1</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="J77" s="3"/>
-      <c r="K77" s="9">
-        <v>10</v>
-      </c>
-      <c r="L77" s="9">
-        <v>10</v>
-      </c>
-      <c r="M77" s="4"/>
-    </row>
-    <row r="78" spans="1:13" ht="16" thickBot="1">
-      <c r="A78" s="3"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="4"/>
-    </row>
-    <row r="79" spans="1:13" ht="53" thickBot="1">
-      <c r="A79" s="3"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="J79" s="26"/>
-      <c r="K79" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L79" s="24">
+      <c r="J69" s="27"/>
+      <c r="K69" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L69" s="15">
         <v>196.09</v>
       </c>
-      <c r="M79" s="23" t="s">
-        <v>318</v>
+      <c r="M69" s="14" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="I69:J69"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -4233,21 +3701,16 @@
     <hyperlink ref="J33" r:id="rId11"/>
     <hyperlink ref="J34" r:id="rId12"/>
     <hyperlink ref="J41" r:id="rId13"/>
-    <hyperlink ref="J42" r:id="rId14"/>
-    <hyperlink ref="J44" r:id="rId15"/>
+    <hyperlink ref="J46" r:id="rId14"/>
+    <hyperlink ref="J47" r:id="rId15"/>
     <hyperlink ref="J48" r:id="rId16"/>
     <hyperlink ref="J49" r:id="rId17"/>
-    <hyperlink ref="J50" r:id="rId18"/>
-    <hyperlink ref="J51" r:id="rId19"/>
-    <hyperlink ref="J52" r:id="rId20"/>
-    <hyperlink ref="J53" r:id="rId21"/>
-    <hyperlink ref="J54" r:id="rId22"/>
-    <hyperlink ref="J64" r:id="rId23"/>
-    <hyperlink ref="J74" r:id="rId24"/>
-    <hyperlink ref="J66" r:id="rId25"/>
+    <hyperlink ref="J64" r:id="rId18"/>
+    <hyperlink ref="J56" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="36" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId20"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Add some missing resistors to the BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.2/schematic v0.2_bom.xlsx
+++ b/reference/hardware/v0.2/schematic v0.2_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="15540" tabRatio="500"/>
@@ -601,9 +601,6 @@
     <t>RES 680 OHM 1/4W 1% AXIAL</t>
   </si>
   <si>
-    <t>R9,12,15,18</t>
-  </si>
-  <si>
     <t>R25,27,31,32</t>
   </si>
   <si>
@@ -746,6 +743,9 @@
   </si>
   <si>
     <t>Can be found much cheaper elsewhere</t>
+  </si>
+  <si>
+    <t>R9,12,15,18,26,28,33,34</t>
   </si>
 </sst>
 </file>
@@ -1381,8 +1381,8 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1462,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -1502,7 +1502,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -1542,7 +1542,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -1582,7 +1582,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>33</v>
@@ -1622,7 +1622,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
@@ -1662,7 +1662,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>44</v>
@@ -1702,7 +1702,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>49</v>
@@ -1774,7 +1774,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>55</v>
@@ -1814,7 +1814,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>62</v>
@@ -1854,16 +1854,16 @@
         <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1884,7 +1884,7 @@
         <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>70</v>
@@ -2047,14 +2047,14 @@
         <v>86</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K21" s="8">
         <v>0.12</v>
@@ -2105,7 +2105,7 @@
         <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>89</v>
@@ -2134,7 +2134,7 @@
         <v>6.22</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16" thickBot="1">
@@ -2174,10 +2174,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>95</v>
@@ -2199,7 +2199,7 @@
         <v>95</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K27" s="9">
         <v>1.75</v>
@@ -2215,16 +2215,16 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>154</v>
@@ -2237,10 +2237,10 @@
         <v>98</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K28" s="9">
         <v>1.79</v>
@@ -2291,7 +2291,7 @@
         <v>100</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>101</v>
@@ -2329,7 +2329,7 @@
         <v>106</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>107</v>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>180</v>
@@ -2582,7 +2582,7 @@
         <v>139</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>140</v>
@@ -2620,7 +2620,7 @@
         <v>144</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D40" s="3">
         <v>160</v>
@@ -2766,14 +2766,14 @@
         <v>160</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G45" s="3">
         <v>1</v>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K45" s="9">
         <v>16.37</v>
@@ -2802,16 +2802,16 @@
         <v>161</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="G46" s="3">
         <v>2</v>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K46" s="8">
         <v>1.98</v>
@@ -2840,16 +2840,16 @@
         <v>163</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="E47" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="G47" s="3">
         <f>A47</f>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K47" s="8">
         <v>1.96</v>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2885,10 +2885,10 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2917,7 +2917,7 @@
         <v>166</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
@@ -2984,10 +2984,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>172</v>
@@ -3018,10 +3018,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3030,7 +3030,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K54" s="3">
         <v>61.65</v>
@@ -3040,7 +3040,7 @@
         <v>61.65</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Fix for typo in v0.2 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.2/schematic v0.2_bom.xlsx
+++ b/reference/hardware/v0.2/schematic v0.2_bom.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="230">
   <si>
     <t>QTY</t>
   </si>
@@ -593,9 +593,6 @@
   </si>
   <si>
     <t>R21</t>
-  </si>
-  <si>
-    <t>680k</t>
   </si>
   <si>
     <t>RES 680 OHM 1/4W 1% AXIAL</t>
@@ -919,9 +916,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1022,7 +1021,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1046,6 +1045,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1381,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1462,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -1502,7 +1503,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -1542,7 +1543,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -1582,7 +1583,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>33</v>
@@ -1622,7 +1623,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
@@ -1662,7 +1663,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>44</v>
@@ -1702,7 +1703,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>49</v>
@@ -1774,7 +1775,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>55</v>
@@ -1814,7 +1815,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>62</v>
@@ -1854,16 +1855,16 @@
         <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1884,7 +1885,7 @@
         <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>70</v>
@@ -2047,14 +2048,14 @@
         <v>86</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K21" s="8">
         <v>0.12</v>
@@ -2105,7 +2106,7 @@
         <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>89</v>
@@ -2134,7 +2135,7 @@
         <v>6.22</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16" thickBot="1">
@@ -2174,10 +2175,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>95</v>
@@ -2199,7 +2200,7 @@
         <v>95</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K27" s="9">
         <v>1.75</v>
@@ -2215,16 +2216,16 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>154</v>
@@ -2237,10 +2238,10 @@
         <v>98</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K28" s="9">
         <v>1.79</v>
@@ -2291,7 +2292,7 @@
         <v>100</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>101</v>
@@ -2329,7 +2330,7 @@
         <v>106</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>107</v>
@@ -2365,13 +2366,13 @@
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="D33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" s="18">
+        <v>680</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="18">
@@ -2582,7 +2583,7 @@
         <v>139</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>140</v>
@@ -2620,7 +2621,7 @@
         <v>144</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D40" s="3">
         <v>160</v>
@@ -2766,14 +2767,14 @@
         <v>160</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G45" s="3">
         <v>1</v>
@@ -2783,7 +2784,7 @@
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K45" s="9">
         <v>16.37</v>
@@ -2802,16 +2803,16 @@
         <v>161</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="G46" s="3">
         <v>2</v>
@@ -2821,7 +2822,7 @@
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K46" s="8">
         <v>1.98</v>
@@ -2840,16 +2841,16 @@
         <v>163</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>219</v>
-      </c>
       <c r="E47" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="G47" s="3">
         <f>A47</f>
@@ -2860,7 +2861,7 @@
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K47" s="8">
         <v>1.96</v>
@@ -2877,7 +2878,7 @@
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2885,10 +2886,10 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2917,7 +2918,7 @@
         <v>166</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
@@ -2984,10 +2985,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>172</v>
@@ -3018,10 +3019,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3030,7 +3031,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K54" s="3">
         <v>61.65</v>
@@ -3040,7 +3041,7 @@
         <v>61.65</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="16" thickBot="1">

</xml_diff>